<commit_message>
Documento do projeto e Analytics atualizado
</commit_message>
<xml_diff>
--- a/arq-comp/Segundo-analytics.xlsx
+++ b/arq-comp/Segundo-analytics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Sprint\GroonTec\arq-comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97CB639-3B04-4825-BC12-746C27D1F3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB01C94-0EC0-4385-AFAD-FA4AD322F155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D1515E8D-A832-4392-92D9-9E5E22F6EFEF}"/>
   </bookViews>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -126,42 +117,15 @@
     <t>Aceitável</t>
   </si>
   <si>
-    <t>400lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>450lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>500lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>600lm&lt; entrada</t>
-  </si>
-  <si>
     <t>Camomila</t>
   </si>
   <si>
     <t>Luminosidade 10:00-14:00</t>
   </si>
   <si>
-    <t>800lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>850lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>900lm&gt;entrada</t>
-  </si>
-  <si>
-    <t>900lm&lt; entrada</t>
-  </si>
-  <si>
     <t>Luminosidade 18:00-6:00</t>
   </si>
   <si>
-    <t>190lm&gt;entrada</t>
-  </si>
-  <si>
     <t>entrada&gt;300</t>
   </si>
   <si>
@@ -208,6 +172,33 @@
   </si>
   <si>
     <t>18-6h (Período Noturno)</t>
+  </si>
+  <si>
+    <t>400&gt;entrada</t>
+  </si>
+  <si>
+    <t>450&gt;entrada</t>
+  </si>
+  <si>
+    <t>500&gt;entrada</t>
+  </si>
+  <si>
+    <t>800&gt;entrada</t>
+  </si>
+  <si>
+    <t>850&gt;entrada</t>
+  </si>
+  <si>
+    <t>900&gt;entrada</t>
+  </si>
+  <si>
+    <t>600 &lt; entrada</t>
+  </si>
+  <si>
+    <t>900 &lt; entrada</t>
+  </si>
+  <si>
+    <t>190 &gt; entrada</t>
   </si>
 </sst>
 </file>
@@ -474,19 +465,25 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -510,37 +507,31 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3053,15 +3044,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>242886</xdr:colOff>
+      <xdr:colOff>7563</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3088,16 +3079,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28295</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>17088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>461402</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>93288</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3427,8 +3418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E8C567-5340-4CA4-8DE6-83689C997126}">
   <dimension ref="B2:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P70" sqref="P70"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC27" sqref="AB27:AC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,29 +3443,29 @@
     <col min="18" max="18" width="15.140625" customWidth="1"/>
     <col min="19" max="19" width="15" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.85546875" customWidth="1"/>
     <col min="25" max="25" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="R2" s="36" t="s">
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="R2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="38"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="26"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -3523,10 +3514,10 @@
       <c r="T3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="32"/>
+      <c r="V3" s="34"/>
       <c r="W3" s="17" t="s">
         <v>12</v>
       </c>
@@ -3538,21 +3529,21 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="F4" s="24" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="F4" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="J4" s="24" t="s">
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="J4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
       <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
@@ -3592,24 +3583,24 @@
       <c r="B5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="27"/>
+      <c r="H5" s="44"/>
       <c r="J5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="27"/>
+      <c r="L5" s="44"/>
       <c r="N5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3620,37 +3611,37 @@
       <c r="P5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="42">
         <v>23</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="42"/>
       <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="42">
         <v>17</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="42"/>
       <c r="J6" s="10">
         <v>1</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="42">
         <v>18</v>
       </c>
-      <c r="L6" s="24"/>
+      <c r="L6" s="42"/>
       <c r="N6" s="3" t="s">
         <v>23</v>
       </c>
@@ -3661,39 +3652,39 @@
       <c r="P6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="36" t="s">
+      <c r="R6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="38"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="26"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="42">
         <v>20</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="42"/>
       <c r="F7" s="10">
         <v>2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="42">
         <v>19</v>
       </c>
-      <c r="H7" s="24"/>
+      <c r="H7" s="42"/>
       <c r="J7" s="10">
         <v>2</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="42">
         <v>18.5</v>
       </c>
-      <c r="L7" s="24"/>
+      <c r="L7" s="42"/>
       <c r="N7" s="3" t="s">
         <v>24</v>
       </c>
@@ -3713,10 +3704,10 @@
       <c r="T7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="32" t="s">
+      <c r="U7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="32"/>
+      <c r="V7" s="34"/>
       <c r="W7" s="17" t="s">
         <v>12</v>
       </c>
@@ -3731,24 +3722,24 @@
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="42">
         <v>18</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="42"/>
       <c r="F8" s="10">
         <v>3</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="42">
         <v>22</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="42"/>
       <c r="J8" s="10">
         <v>3</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="42">
         <v>19</v>
       </c>
-      <c r="L8" s="24"/>
+      <c r="L8" s="42"/>
       <c r="N8" s="3" t="s">
         <v>25</v>
       </c>
@@ -3788,93 +3779,93 @@
       <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="42">
         <v>28</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="42"/>
       <c r="F9" s="10">
         <v>4</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="42">
         <v>23</v>
       </c>
-      <c r="H9" s="24"/>
+      <c r="H9" s="42"/>
       <c r="J9" s="10">
         <v>4</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="42">
         <v>19</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
+      <c r="L9" s="42"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="42">
         <v>25</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="42"/>
       <c r="F10" s="10">
         <v>5</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="42">
         <v>20</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="42"/>
       <c r="J10" s="10">
         <v>5</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="42">
         <v>19.5</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="N10" s="25" t="s">
+      <c r="L10" s="42"/>
+      <c r="N10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="R10" s="36" t="s">
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="R10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37"/>
-      <c r="V10" s="37"/>
-      <c r="W10" s="37"/>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="38"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="26"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>6</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="42">
         <v>31</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="42"/>
       <c r="F11" s="10">
         <v>6</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="42">
         <v>26</v>
       </c>
-      <c r="H11" s="24"/>
+      <c r="H11" s="42"/>
       <c r="J11" s="10">
         <v>6</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="42">
         <v>20</v>
       </c>
-      <c r="L11" s="24"/>
+      <c r="L11" s="42"/>
       <c r="N11" s="15" t="s">
         <v>8</v>
       </c>
@@ -3894,10 +3885,10 @@
       <c r="T11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U11" s="32" t="s">
+      <c r="U11" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="V11" s="32"/>
+      <c r="V11" s="34"/>
       <c r="W11" s="17" t="s">
         <v>12</v>
       </c>
@@ -3912,24 +3903,24 @@
       <c r="B12" s="10">
         <v>7</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="42">
         <v>37</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="42"/>
       <c r="F12" s="10">
         <v>7</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="42">
         <v>27</v>
       </c>
-      <c r="H12" s="24"/>
+      <c r="H12" s="42"/>
       <c r="J12" s="10">
         <v>7</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="42">
         <v>20</v>
       </c>
-      <c r="L12" s="24"/>
+      <c r="L12" s="42"/>
       <c r="N12" s="16" t="s">
         <v>27</v>
       </c>
@@ -3969,24 +3960,24 @@
       <c r="B13" s="10">
         <v>8</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="42">
         <v>35</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="42"/>
       <c r="F13" s="10">
         <v>8</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="42">
         <v>30</v>
       </c>
-      <c r="H13" s="24"/>
+      <c r="H13" s="42"/>
       <c r="J13" s="10">
         <v>8</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="42">
         <v>21</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="42"/>
       <c r="N13" s="16" t="s">
         <v>3</v>
       </c>
@@ -3997,37 +3988,37 @@
       <c r="P13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="45"/>
-      <c r="X13" s="45"/>
-      <c r="Y13" s="45"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>9</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="42">
         <v>40</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="42"/>
       <c r="F14" s="10">
         <v>9</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="42">
         <v>33</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="42"/>
       <c r="J14" s="10">
         <v>9</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="42">
         <v>21.5</v>
       </c>
-      <c r="L14" s="24"/>
+      <c r="L14" s="42"/>
       <c r="N14" s="16" t="s">
         <v>23</v>
       </c>
@@ -4038,37 +4029,37 @@
       <c r="P14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="46"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>10</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="42">
         <v>38</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="42"/>
       <c r="F15" s="10">
         <v>10</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="42">
         <v>35</v>
       </c>
-      <c r="H15" s="24"/>
+      <c r="H15" s="42"/>
       <c r="J15" s="10">
         <v>10</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="42">
         <v>21</v>
       </c>
-      <c r="L15" s="24"/>
+      <c r="L15" s="42"/>
       <c r="N15" s="16" t="s">
         <v>24</v>
       </c>
@@ -4079,40 +4070,40 @@
       <c r="P15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R15" s="36" t="s">
+      <c r="R15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="38"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="26"/>
       <c r="AB15" s="14"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>11</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="42">
         <v>31</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="42"/>
       <c r="F16" s="10">
         <v>11</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="42">
         <v>32</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="42"/>
       <c r="J16" s="10">
         <v>11</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="42">
         <v>22</v>
       </c>
-      <c r="L16" s="24"/>
+      <c r="L16" s="42"/>
       <c r="N16" s="16" t="s">
         <v>25</v>
       </c>
@@ -4132,114 +4123,114 @@
       <c r="T16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U16" s="39" t="s">
+      <c r="U16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="V16" s="40"/>
-      <c r="W16" s="40"/>
-      <c r="X16" s="40"/>
-      <c r="Y16" s="41"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="29"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>12</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="42">
         <v>29</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="42"/>
       <c r="F17" s="10">
         <v>12</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="42">
         <v>30</v>
       </c>
-      <c r="H17" s="24"/>
+      <c r="H17" s="42"/>
       <c r="J17" s="10">
         <v>12</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="42">
         <v>20</v>
       </c>
-      <c r="L17" s="24"/>
+      <c r="L17" s="42"/>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
       <c r="R17" s="18" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="S17" s="19" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="T17" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="U17" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="35"/>
+        <v>51</v>
+      </c>
+      <c r="U17" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="37"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>13</v>
       </c>
-      <c r="C18" s="24">
+      <c r="C18" s="42">
         <v>24</v>
       </c>
-      <c r="D18" s="24"/>
+      <c r="D18" s="42"/>
       <c r="F18" s="10">
         <v>13</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="42">
         <v>27</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="42"/>
       <c r="J18" s="10">
         <v>13</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="42">
         <v>19.5</v>
       </c>
-      <c r="L18" s="24"/>
-      <c r="N18" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
-      <c r="U18" s="44"/>
-      <c r="V18" s="44"/>
-      <c r="W18" s="44"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="44"/>
+      <c r="L18" s="42"/>
+      <c r="N18" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>14</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="42">
         <v>21</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="42"/>
       <c r="F19" s="10">
         <v>14</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="42">
         <v>24</v>
       </c>
-      <c r="H19" s="24"/>
+      <c r="H19" s="42"/>
       <c r="J19" s="10">
         <v>14</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="42">
         <v>19</v>
       </c>
-      <c r="L19" s="24"/>
+      <c r="L19" s="42"/>
       <c r="N19" s="16" t="s">
         <v>8</v>
       </c>
@@ -4250,39 +4241,39 @@
       <c r="P19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R19" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="38"/>
+      <c r="R19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="26"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>15</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C20" s="42">
         <v>20</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="42"/>
       <c r="F20" s="10">
         <v>15</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="42">
         <v>19</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="42"/>
       <c r="J20" s="10">
         <v>15</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="42">
         <v>18</v>
       </c>
-      <c r="L20" s="24"/>
+      <c r="L20" s="42"/>
       <c r="N20" s="16" t="s">
         <v>27</v>
       </c>
@@ -4302,13 +4293,13 @@
       <c r="T20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="U20" s="39" t="s">
+      <c r="U20" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="V20" s="40"/>
-      <c r="W20" s="40"/>
-      <c r="X20" s="40"/>
-      <c r="Y20" s="41"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="29"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N21" s="16" t="s">
@@ -4322,21 +4313,21 @@
         <v>13</v>
       </c>
       <c r="R21" s="18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="T21" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="U21" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="35"/>
+        <v>54</v>
+      </c>
+      <c r="U21" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="37"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N22" s="16" t="s">
@@ -4349,14 +4340,14 @@
       <c r="P22" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="44"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N23" s="16" t="s">
@@ -4369,16 +4360,16 @@
       <c r="P23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R23" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="38"/>
+      <c r="R23" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="26"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="N24" s="16" t="s">
@@ -4391,13 +4382,13 @@
       <c r="P24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R24" s="42" t="s">
+      <c r="R24" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="42"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
       <c r="W24" s="17" t="s">
         <v>12</v>
       </c>
@@ -4412,21 +4403,21 @@
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
-      <c r="R25" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
+      <c r="R25" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
       <c r="W25" s="20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="X25" s="23" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="Y25" s="18" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
@@ -4434,73 +4425,73 @@
     </row>
     <row r="38" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="P38" s="10" t="s">
         <v>3</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S38" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="T38" s="30"/>
-      <c r="U38" s="31"/>
-      <c r="W38" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="S38" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="T38" s="32"/>
+      <c r="U38" s="33"/>
+      <c r="W38" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="33"/>
     </row>
     <row r="39" spans="3:25" x14ac:dyDescent="0.25">
-      <c r="C39" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="G39" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="K39" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="O39" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
+      <c r="C39" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="G39" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="K39" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="42"/>
+      <c r="M39" s="42"/>
+      <c r="O39" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="P39" s="42"/>
+      <c r="Q39" s="42"/>
       <c r="S39" s="4" t="s">
         <v>8</v>
       </c>
@@ -4524,33 +4515,33 @@
     </row>
     <row r="40" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="44"/>
       <c r="G40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="H40" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="I40" s="44"/>
       <c r="K40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L40" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="M40" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="L40" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="M40" s="44"/>
       <c r="O40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="P40" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q40" s="27"/>
+        <v>46</v>
+      </c>
+      <c r="P40" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q40" s="44"/>
       <c r="S40" s="3" t="s">
         <v>27</v>
       </c>
@@ -4576,31 +4567,31 @@
       <c r="C41" s="10">
         <v>1</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="42">
         <v>450</v>
       </c>
-      <c r="E41" s="24"/>
+      <c r="E41" s="42"/>
       <c r="G41" s="10">
         <v>1</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="42">
         <v>800</v>
       </c>
-      <c r="I41" s="24"/>
+      <c r="I41" s="42"/>
       <c r="K41" s="10">
         <v>1</v>
       </c>
-      <c r="L41" s="24">
+      <c r="L41" s="42">
         <v>400</v>
       </c>
-      <c r="M41" s="24"/>
+      <c r="M41" s="42"/>
       <c r="O41" s="10">
         <v>1</v>
       </c>
-      <c r="P41" s="24">
+      <c r="P41" s="42">
         <v>50</v>
       </c>
-      <c r="Q41" s="24"/>
+      <c r="Q41" s="42"/>
       <c r="S41" s="3" t="s">
         <v>3</v>
       </c>
@@ -4626,31 +4617,31 @@
       <c r="C42" s="10">
         <v>2</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="42">
         <v>500</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="42"/>
       <c r="G42" s="10">
         <v>2</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="42">
         <v>850</v>
       </c>
-      <c r="I42" s="24"/>
+      <c r="I42" s="42"/>
       <c r="K42" s="10">
         <v>2</v>
       </c>
-      <c r="L42" s="24">
+      <c r="L42" s="42">
         <v>500</v>
       </c>
-      <c r="M42" s="24"/>
+      <c r="M42" s="42"/>
       <c r="O42" s="10">
         <v>2</v>
       </c>
-      <c r="P42" s="24">
+      <c r="P42" s="42">
         <v>100</v>
       </c>
-      <c r="Q42" s="24"/>
+      <c r="Q42" s="42"/>
       <c r="S42" s="3" t="s">
         <v>23</v>
       </c>
@@ -4676,31 +4667,31 @@
       <c r="C43" s="10">
         <v>3</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="42">
         <v>550</v>
       </c>
-      <c r="E43" s="24"/>
+      <c r="E43" s="42"/>
       <c r="G43" s="10">
         <v>3</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="42">
         <v>900</v>
       </c>
-      <c r="I43" s="24"/>
+      <c r="I43" s="42"/>
       <c r="K43" s="10">
         <v>3</v>
       </c>
-      <c r="L43" s="24">
+      <c r="L43" s="42">
         <v>470</v>
       </c>
-      <c r="M43" s="24"/>
+      <c r="M43" s="42"/>
       <c r="O43" s="10">
         <v>3</v>
       </c>
-      <c r="P43" s="24">
+      <c r="P43" s="42">
         <v>50</v>
       </c>
-      <c r="Q43" s="24"/>
+      <c r="Q43" s="42"/>
       <c r="S43" s="3" t="s">
         <v>24</v>
       </c>
@@ -4726,31 +4717,31 @@
       <c r="C44" s="10">
         <v>4</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="42">
         <v>640</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="42"/>
       <c r="G44" s="10">
         <v>4</v>
       </c>
-      <c r="H44" s="24">
+      <c r="H44" s="42">
         <v>930</v>
       </c>
-      <c r="I44" s="24"/>
+      <c r="I44" s="42"/>
       <c r="K44" s="10">
         <v>4</v>
       </c>
-      <c r="L44" s="24">
+      <c r="L44" s="42">
         <v>556</v>
       </c>
-      <c r="M44" s="24"/>
+      <c r="M44" s="42"/>
       <c r="O44" s="10">
         <v>4</v>
       </c>
-      <c r="P44" s="24">
+      <c r="P44" s="42">
         <v>400</v>
       </c>
-      <c r="Q44" s="24"/>
+      <c r="Q44" s="42"/>
       <c r="S44" s="3" t="s">
         <v>25</v>
       </c>
@@ -4776,101 +4767,101 @@
       <c r="C45" s="10">
         <v>5</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="42">
         <v>650</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="42"/>
       <c r="G45" s="10">
         <v>5</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H45" s="42">
         <v>1000</v>
       </c>
-      <c r="I45" s="24"/>
+      <c r="I45" s="42"/>
       <c r="K45" s="10">
         <v>5</v>
       </c>
-      <c r="L45" s="24">
+      <c r="L45" s="42">
         <v>600</v>
       </c>
-      <c r="M45" s="24"/>
+      <c r="M45" s="42"/>
       <c r="O45" s="10">
         <v>5</v>
       </c>
-      <c r="P45" s="24">
+      <c r="P45" s="42">
         <v>310</v>
       </c>
-      <c r="Q45" s="24"/>
+      <c r="Q45" s="42"/>
     </row>
     <row r="46" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C46" s="10">
         <v>6</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="42">
         <v>600</v>
       </c>
-      <c r="E46" s="24"/>
+      <c r="E46" s="42"/>
       <c r="G46" s="10">
         <v>6</v>
       </c>
-      <c r="H46" s="24">
+      <c r="H46" s="42">
         <v>940</v>
       </c>
-      <c r="I46" s="24"/>
+      <c r="I46" s="42"/>
       <c r="K46" s="10">
         <v>6</v>
       </c>
-      <c r="L46" s="24">
+      <c r="L46" s="42">
         <v>620</v>
       </c>
-      <c r="M46" s="24"/>
+      <c r="M46" s="42"/>
       <c r="O46" s="10">
         <v>6</v>
       </c>
-      <c r="P46" s="24">
+      <c r="P46" s="42">
         <v>350</v>
       </c>
-      <c r="Q46" s="24"/>
-      <c r="S46" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="T46" s="30"/>
-      <c r="U46" s="31"/>
-      <c r="W46" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="31"/>
+      <c r="Q46" s="42"/>
+      <c r="S46" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="T46" s="32"/>
+      <c r="U46" s="33"/>
+      <c r="W46" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="33"/>
     </row>
     <row r="47" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C47" s="10">
         <v>7</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="42">
         <v>700</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="42"/>
       <c r="G47" s="10">
         <v>7</v>
       </c>
-      <c r="H47" s="24">
+      <c r="H47" s="42">
         <v>840</v>
       </c>
-      <c r="I47" s="24"/>
+      <c r="I47" s="42"/>
       <c r="K47" s="10">
         <v>7</v>
       </c>
-      <c r="L47" s="24">
+      <c r="L47" s="42">
         <v>680</v>
       </c>
-      <c r="M47" s="24"/>
+      <c r="M47" s="42"/>
       <c r="O47" s="10">
         <v>7</v>
       </c>
-      <c r="P47" s="24">
+      <c r="P47" s="42">
         <v>200</v>
       </c>
-      <c r="Q47" s="24"/>
+      <c r="Q47" s="42"/>
       <c r="S47" s="4" t="s">
         <v>8</v>
       </c>
@@ -4896,31 +4887,31 @@
       <c r="C48" s="10">
         <v>8</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="42">
         <v>750</v>
       </c>
-      <c r="E48" s="24"/>
+      <c r="E48" s="42"/>
       <c r="G48" s="10">
         <v>8</v>
       </c>
-      <c r="H48" s="24">
+      <c r="H48" s="42">
         <v>820</v>
       </c>
-      <c r="I48" s="24"/>
+      <c r="I48" s="42"/>
       <c r="K48" s="10">
         <v>8</v>
       </c>
-      <c r="L48" s="24">
+      <c r="L48" s="42">
         <v>740</v>
       </c>
-      <c r="M48" s="24"/>
+      <c r="M48" s="42"/>
       <c r="O48" s="10">
         <v>8</v>
       </c>
-      <c r="P48" s="24">
+      <c r="P48" s="42">
         <v>150</v>
       </c>
-      <c r="Q48" s="24"/>
+      <c r="Q48" s="42"/>
       <c r="S48" s="3" t="s">
         <v>27</v>
       </c>
@@ -4946,31 +4937,31 @@
       <c r="C49" s="10">
         <v>9</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="42">
         <v>800</v>
       </c>
-      <c r="E49" s="24"/>
+      <c r="E49" s="42"/>
       <c r="G49" s="10">
         <v>9</v>
       </c>
-      <c r="H49" s="24">
+      <c r="H49" s="42">
         <v>960</v>
       </c>
-      <c r="I49" s="24"/>
+      <c r="I49" s="42"/>
       <c r="K49" s="10">
         <v>9</v>
       </c>
-      <c r="L49" s="24">
+      <c r="L49" s="42">
         <v>700</v>
       </c>
-      <c r="M49" s="24"/>
+      <c r="M49" s="42"/>
       <c r="O49" s="10">
         <v>9</v>
       </c>
-      <c r="P49" s="24">
+      <c r="P49" s="42">
         <v>70</v>
       </c>
-      <c r="Q49" s="24"/>
+      <c r="Q49" s="42"/>
       <c r="S49" s="3" t="s">
         <v>3</v>
       </c>
@@ -4996,31 +4987,31 @@
       <c r="C50" s="10">
         <v>10</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="42">
         <v>470</v>
       </c>
-      <c r="E50" s="24"/>
+      <c r="E50" s="42"/>
       <c r="G50" s="10">
         <v>10</v>
       </c>
-      <c r="H50" s="24">
+      <c r="H50" s="42">
         <v>1000</v>
       </c>
-      <c r="I50" s="24"/>
+      <c r="I50" s="42"/>
       <c r="K50" s="10">
         <v>10</v>
       </c>
-      <c r="L50" s="24">
+      <c r="L50" s="42">
         <v>460</v>
       </c>
-      <c r="M50" s="24"/>
+      <c r="M50" s="42"/>
       <c r="O50" s="10">
         <v>10</v>
       </c>
-      <c r="P50" s="24">
+      <c r="P50" s="42">
         <v>300</v>
       </c>
-      <c r="Q50" s="24"/>
+      <c r="Q50" s="42"/>
       <c r="S50" s="3" t="s">
         <v>23</v>
       </c>
@@ -5046,31 +5037,31 @@
       <c r="C51" s="10">
         <v>11</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="42">
         <v>540</v>
       </c>
-      <c r="E51" s="24"/>
+      <c r="E51" s="42"/>
       <c r="G51" s="10">
         <v>11</v>
       </c>
-      <c r="H51" s="24">
+      <c r="H51" s="42">
         <v>930</v>
       </c>
-      <c r="I51" s="24"/>
+      <c r="I51" s="42"/>
       <c r="K51" s="10">
         <v>11</v>
       </c>
-      <c r="L51" s="28">
+      <c r="L51" s="45">
         <v>800</v>
       </c>
-      <c r="M51" s="28"/>
+      <c r="M51" s="45"/>
       <c r="O51" s="10">
         <v>11</v>
       </c>
-      <c r="P51" s="24">
+      <c r="P51" s="42">
         <v>250</v>
       </c>
-      <c r="Q51" s="24"/>
+      <c r="Q51" s="42"/>
       <c r="S51" s="3" t="s">
         <v>24</v>
       </c>
@@ -5096,31 +5087,31 @@
       <c r="C52" s="10">
         <v>12</v>
       </c>
-      <c r="D52" s="24">
+      <c r="D52" s="42">
         <v>630</v>
       </c>
-      <c r="E52" s="24"/>
+      <c r="E52" s="42"/>
       <c r="G52" s="10">
         <v>12</v>
       </c>
-      <c r="H52" s="24">
+      <c r="H52" s="42">
         <v>830</v>
       </c>
-      <c r="I52" s="24"/>
+      <c r="I52" s="42"/>
       <c r="K52" s="10">
         <v>12</v>
       </c>
-      <c r="L52" s="24">
+      <c r="L52" s="42">
         <v>570</v>
       </c>
-      <c r="M52" s="24"/>
+      <c r="M52" s="42"/>
       <c r="O52" s="10">
         <v>12</v>
       </c>
-      <c r="P52" s="24">
+      <c r="P52" s="42">
         <v>60</v>
       </c>
-      <c r="Q52" s="24"/>
+      <c r="Q52" s="42"/>
       <c r="S52" s="3" t="s">
         <v>25</v>
       </c>
@@ -5146,153 +5137,157 @@
       <c r="C53" s="10">
         <v>13</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53" s="42">
         <v>750</v>
       </c>
-      <c r="E53" s="24"/>
+      <c r="E53" s="42"/>
       <c r="G53" s="10">
         <v>13</v>
       </c>
-      <c r="H53" s="24">
+      <c r="H53" s="42">
         <v>920</v>
       </c>
-      <c r="I53" s="24"/>
+      <c r="I53" s="42"/>
       <c r="K53" s="10">
         <v>13</v>
       </c>
-      <c r="L53" s="24">
+      <c r="L53" s="42">
         <v>790</v>
       </c>
-      <c r="M53" s="24"/>
+      <c r="M53" s="42"/>
       <c r="O53" s="10">
         <v>13</v>
       </c>
-      <c r="P53" s="24">
+      <c r="P53" s="42">
         <v>370</v>
       </c>
-      <c r="Q53" s="24"/>
+      <c r="Q53" s="42"/>
     </row>
     <row r="54" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C54" s="10">
         <v>14</v>
       </c>
-      <c r="D54" s="24">
+      <c r="D54" s="42">
         <v>400</v>
       </c>
-      <c r="E54" s="24"/>
+      <c r="E54" s="42"/>
       <c r="G54" s="10">
         <v>14</v>
       </c>
-      <c r="H54" s="24">
+      <c r="H54" s="42">
         <v>940</v>
       </c>
-      <c r="I54" s="24"/>
+      <c r="I54" s="42"/>
       <c r="K54" s="10">
         <v>14</v>
       </c>
-      <c r="L54" s="24">
+      <c r="L54" s="42">
         <v>730</v>
       </c>
-      <c r="M54" s="24"/>
+      <c r="M54" s="42"/>
       <c r="O54" s="10">
         <v>14</v>
       </c>
-      <c r="P54" s="24">
+      <c r="P54" s="42">
         <v>190</v>
       </c>
-      <c r="Q54" s="24"/>
+      <c r="Q54" s="42"/>
     </row>
     <row r="55" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C55" s="10">
         <v>15</v>
       </c>
-      <c r="D55" s="24">
+      <c r="D55" s="42">
         <v>590</v>
       </c>
-      <c r="E55" s="24"/>
+      <c r="E55" s="42"/>
       <c r="G55" s="10">
         <v>15</v>
       </c>
-      <c r="H55" s="24">
+      <c r="H55" s="42">
         <v>900</v>
       </c>
-      <c r="I55" s="24"/>
+      <c r="I55" s="42"/>
       <c r="K55" s="10">
         <v>15</v>
       </c>
-      <c r="L55" s="24">
+      <c r="L55" s="42">
         <v>450</v>
       </c>
-      <c r="M55" s="24"/>
+      <c r="M55" s="42"/>
       <c r="O55" s="10">
         <v>15</v>
       </c>
-      <c r="P55" s="24">
+      <c r="P55" s="42">
         <v>80</v>
       </c>
-      <c r="Q55" s="24"/>
+      <c r="Q55" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="146">
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="R6:Y6"/>
-    <mergeCell ref="R10:Y10"/>
-    <mergeCell ref="R15:Y15"/>
-    <mergeCell ref="U16:Y16"/>
-    <mergeCell ref="R5:Y5"/>
-    <mergeCell ref="W38:Y38"/>
-    <mergeCell ref="W46:Y46"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="R19:Y19"/>
-    <mergeCell ref="U20:Y20"/>
-    <mergeCell ref="U21:Y21"/>
-    <mergeCell ref="R23:Y23"/>
-    <mergeCell ref="R24:V24"/>
-    <mergeCell ref="R25:V25"/>
-    <mergeCell ref="R9:Y9"/>
-    <mergeCell ref="R13:Y14"/>
-    <mergeCell ref="R18:Y18"/>
-    <mergeCell ref="R22:Y22"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="S38:U38"/>
-    <mergeCell ref="S46:U46"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="P51:Q51"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="P53:Q53"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="L53:M53"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="L55:M55"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="L48:M48"/>
     <mergeCell ref="L49:M49"/>
     <mergeCell ref="L50:M50"/>
@@ -5317,69 +5312,65 @@
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L53:M53"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="L55:M55"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="S38:U38"/>
+    <mergeCell ref="S46:U46"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="R6:Y6"/>
+    <mergeCell ref="R10:Y10"/>
+    <mergeCell ref="R15:Y15"/>
+    <mergeCell ref="U16:Y16"/>
+    <mergeCell ref="R5:Y5"/>
+    <mergeCell ref="W38:Y38"/>
+    <mergeCell ref="W46:Y46"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="R19:Y19"/>
+    <mergeCell ref="U20:Y20"/>
+    <mergeCell ref="U21:Y21"/>
+    <mergeCell ref="R23:Y23"/>
+    <mergeCell ref="R24:V24"/>
+    <mergeCell ref="R25:V25"/>
+    <mergeCell ref="R9:Y9"/>
+    <mergeCell ref="R13:Y14"/>
+    <mergeCell ref="R18:Y18"/>
+    <mergeCell ref="R22:Y22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5397,12 +5388,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A5FC0246A07B443A05063C8EB2AC7D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="66c8509e2b56534c9610dde05e7b52df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8061e086-846d-4709-83ef-f95cce98977c" xmlns:ns4="48e10f42-d471-48c1-baae-87061c493778" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9c4fe57077946f9e271eb195b6ff0e6" ns3:_="" ns4:_="">
     <xsd:import namespace="8061e086-846d-4709-83ef-f95cce98977c"/>
@@ -5619,6 +5604,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18658B64-C2C7-44AC-9AE6-B8704F93B302}">
   <ds:schemaRefs>
@@ -5628,15 +5619,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9201240-A624-464D-9983-95E53EB343A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9CF7863-B20A-4345-ADEB-8A7C8DDAA280}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5653,4 +5635,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9201240-A624-464D-9983-95E53EB343A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>